<commit_message>
The previous commit is a great example of why testing is a good thing.
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/xlsx_export/Table_3.xlsx
+++ b/tests/testthat/_snaps/xlsx_export/Table_3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">species</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tholothian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a footnote.</t>
   </si>
 </sst>
 </file>
@@ -64,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -83,6 +86,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -92,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -156,11 +164,25 @@
         <color rgb="FF99C199"/>
       </bottom>
     </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -172,6 +194,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -494,16 +519,16 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -514,16 +539,16 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="n">
+      <c r="C2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -534,16 +559,16 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="n">
+      <c r="C3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -554,16 +579,16 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="n">
+      <c r="C4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -574,16 +599,16 @@
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="n">
+      <c r="C5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -594,16 +619,16 @@
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="n">
+      <c r="C6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -614,16 +639,16 @@
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="n">
+      <c r="C7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -634,16 +659,16 @@
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7" t="n">
+      <c r="C8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -654,16 +679,16 @@
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7" t="n">
+      <c r="C9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -674,16 +699,16 @@
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="n">
+      <c r="C10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -694,16 +719,16 @@
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7" t="n">
+      <c r="C11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -714,16 +739,16 @@
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="n">
+      <c r="C12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -734,16 +759,16 @@
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="7" t="n">
+      <c r="C13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -754,16 +779,16 @@
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7" t="n">
+      <c r="C14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -774,16 +799,16 @@
       <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7" t="n">
+      <c r="D15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -794,16 +819,16 @@
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="8" t="n">
         <v>6</v>
       </c>
     </row>
@@ -814,16 +839,16 @@
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7" t="n">
+      <c r="C17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -834,16 +859,16 @@
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7" t="n">
+      <c r="C18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -854,16 +879,16 @@
       <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7" t="n">
+      <c r="C19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7" t="n">
+      <c r="E19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -874,16 +899,16 @@
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7" t="n">
+      <c r="C20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7" t="n">
+      <c r="E20" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -894,16 +919,16 @@
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7" t="n">
+      <c r="C21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -914,16 +939,16 @@
       <c r="B22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7" t="n">
+      <c r="C22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -934,16 +959,16 @@
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7" t="n">
+      <c r="D23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -954,16 +979,16 @@
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7" t="n">
+      <c r="C24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -974,18 +999,28 @@
       <c r="B25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="C25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" ht="27" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Enforcing Arial to make tests pass all platforms.
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/xlsx_export/Table_3.xlsx
+++ b/tests/testthat/_snaps/xlsx_export/Table_3.xlsx
@@ -67,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -85,11 +85,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,7 +191,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">

</xml_diff>